<commit_message>
Updated with ADCON2 = 15 ' Set Negative Reference Setting to ADNREF in ADCON1
</commit_message>
<xml_diff>
--- a/GCBASIC/Tracker/Tracker.xlsx
+++ b/GCBASIC/Tracker/Tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Status</t>
   </si>
@@ -132,6 +132,10 @@
  Goto SetMeasure
  END IF
           See https://sourceforge.net/p/gcbasic/discussion/596084/thread/54c2646f/#1e20</t>
+  </si>
+  <si>
+    <t>New device with an ADC error.  Needs ADCON2 = 15 ' Set Negative Reference Setting to ADNREF in ADCON1 
+See https://sourceforge.net/p/gcbasic/discussion/629990/thread/9b69d693/#e018</t>
   </si>
 </sst>
 </file>
@@ -488,10 +492,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +678,17 @@
       </c>
       <c r="D15" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and closed #16 Added #17. AVR compiler bug.
</commit_message>
<xml_diff>
--- a/GCBASIC/Tracker/Tracker.xlsx
+++ b/GCBASIC/Tracker/Tracker.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Status</t>
   </si>
@@ -136,6 +136,13 @@
   <si>
     <t>New device with an ADC error.  Needs ADCON2 = 15 ' Set Negative Reference Setting to ADNREF in ADCON1 
 See https://sourceforge.net/p/gcbasic/discussion/629990/thread/9b69d693/#e018</t>
+  </si>
+  <si>
+    <t>AVR compiles when it should not.  See https://sourceforge.net/p/gcbasic/discussion/596084/thread/e58866dc/#5e0f</t>
+  </si>
+  <si>
+    <t>HSERPRINT not handling LONGs correctly.
+Updated USART.H to handle LONGs correctly.</t>
   </si>
 </sst>
 </file>
@@ -492,10 +499,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,6 +696,28 @@
       </c>
       <c r="D16" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>